<commit_message>
Added images of phase 2 populated the preference ranking sheet with responses
</commit_message>
<xml_diff>
--- a/ElectrotactileFeedback/Analysis/Phase2presetsheet.xlsx
+++ b/ElectrotactileFeedback/Analysis/Phase2presetsheet.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ae8aac97e7392d0/Documents/Uni/Level 5/Individual Project/Repository/ElectrotactileFeedback/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ae8aac97e7392d0/Documents/Uni/Level 5/Individual Project/Repository/ElectrotactileFeedback/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A14C6BA-202D-4FEE-82B8-D0F6180C3F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{0A14C6BA-202D-4FEE-82B8-D0F6180C3F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A0D698-D99D-4628-838B-737D5B59A057}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E84A4F79-08E3-42E0-B68B-E40380E82165}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E84A4F79-08E3-42E0-B68B-E40380E82165}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>User</t>
   </si>
@@ -60,7 +60,10 @@
     <t>Presets Not Felt</t>
   </si>
   <si>
-    <t>If there were any presets that you could not feel on the final window, please list them here.</t>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
 </sst>
 </file>
@@ -96,13 +99,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -113,6 +123,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -131,11 +145,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{36D235B4-C8DD-4072-AB38-4CE2484F334C}" name="Table3" displayName="Table3" ref="A34:B45" totalsRowShown="0">
-  <autoFilter ref="A34:B45" xr:uid="{36D235B4-C8DD-4072-AB38-4CE2484F334C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{36D235B4-C8DD-4072-AB38-4CE2484F334C}" name="Table3" displayName="Table3" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12" xr:uid="{36D235B4-C8DD-4072-AB38-4CE2484F334C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6F5B3169-A981-46E5-B05E-F32D56E8C823}" name="User"/>
-    <tableColumn id="2" xr3:uid="{2B0C2CCE-8801-42BE-A977-9D7D753B7E06}" name="Presets Not Felt"/>
+    <tableColumn id="2" xr3:uid="{2B0C2CCE-8801-42BE-A977-9D7D753B7E06}" name="Presets Not Felt" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -438,21 +452,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E10A3B-AD49-44B3-A1CD-1C288034CA7F}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.62890625" customWidth="1"/>
-    <col min="2" max="4" width="14.26171875" customWidth="1"/>
-    <col min="5" max="5" width="15.26171875" customWidth="1"/>
-    <col min="6" max="6" width="14.26171875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,175 +486,407 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA265C53-546F-4493-9C28-32D5B2C1D949}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>